<commit_message>
DOCS:  Amalgamate data in master tab of spreadsheet
Amalgamate data in master tab of spreadsheet.  Add observations to challenges in data amalgamation.
</commit_message>
<xml_diff>
--- a/wikipedia_euro_2016_stats.xlsx
+++ b/wikipedia_euro_2016_stats.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27127"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27226"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25080" windowHeight="16060" tabRatio="500" activeTab="5"/>
@@ -1071,7 +1071,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J37"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
@@ -2287,7 +2290,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
@@ -2607,7 +2613,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>

</xml_diff>

<commit_message>
Docs:  update goalkeeper stats
Update goalkeeper stats.
</commit_message>
<xml_diff>
--- a/wikipedia_euro_2016_stats.xlsx
+++ b/wikipedia_euro_2016_stats.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27226"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25080" windowHeight="16060" tabRatio="500" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25080" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="group_stage" sheetId="1" r:id="rId1"/>
@@ -1071,7 +1071,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
@@ -3031,7 +3031,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>

</xml_diff>